<commit_message>
additional fix for training loss
</commit_message>
<xml_diff>
--- a/model_notes.xlsx
+++ b/model_notes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfels\OneDrive\Dokumenter\vae_lung_tumor_segmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8171146B-A515-426F-A56B-14F8ABEB9ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D03FD1-AE72-4478-A2A4-73134AECD6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_notes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="40">
   <si>
     <t>No.</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>(0.9, 0.999)</t>
-  </si>
-  <si>
-    <t>No weight decay -&gt; overfitting</t>
   </si>
   <si>
     <t>(0.8, 0.999)</t>
@@ -148,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -983,11 +980,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1062,7 @@
         <v>36</v>
       </c>
       <c r="R1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T1" t="s">
         <v>15</v>
@@ -1124,7 +1121,7 @@
         <v>37</v>
       </c>
       <c r="R2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T2">
         <v>1.5625</v>
@@ -1183,7 +1180,7 @@
         <v>37</v>
       </c>
       <c r="R3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T3">
         <v>7.8125</v>
@@ -1239,7 +1236,7 @@
         <v>37</v>
       </c>
       <c r="R4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T4">
         <v>15.625</v>
@@ -1295,7 +1292,7 @@
         <v>37</v>
       </c>
       <c r="R5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T5">
         <v>7.8125</v>
@@ -1354,7 +1351,7 @@
         <v>37</v>
       </c>
       <c r="R6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T6">
         <v>7.8125</v>
@@ -1410,7 +1407,7 @@
         <v>37</v>
       </c>
       <c r="R7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T7">
         <v>15.625</v>
@@ -1466,7 +1463,7 @@
         <v>37</v>
       </c>
       <c r="R8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T8">
         <v>15.625</v>
@@ -1516,7 +1513,7 @@
         <v>37</v>
       </c>
       <c r="R9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T9">
         <v>46.875</v>
@@ -1572,7 +1569,7 @@
         <v>37</v>
       </c>
       <c r="R10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T10">
         <v>46.875</v>
@@ -1628,7 +1625,7 @@
         <v>37</v>
       </c>
       <c r="R11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T11">
         <v>11.71875</v>
@@ -1684,7 +1681,7 @@
         <v>37</v>
       </c>
       <c r="R12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T12">
         <v>93.75</v>
@@ -1740,7 +1737,7 @@
         <v>37</v>
       </c>
       <c r="R13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T13">
         <v>93.75</v>
@@ -1793,7 +1790,7 @@
         <v>37</v>
       </c>
       <c r="R14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T14">
         <v>117.1875</v>
@@ -1849,7 +1846,7 @@
         <v>37</v>
       </c>
       <c r="R15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T15">
         <v>19.53125</v>
@@ -1899,7 +1896,7 @@
         <v>37</v>
       </c>
       <c r="R16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T16">
         <v>9.765625</v>
@@ -1955,7 +1952,7 @@
         <v>37</v>
       </c>
       <c r="R17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T17" t="e">
         <v>#DIV/0!</v>
@@ -2010,9 +2007,6 @@
       <c r="Q18" t="s">
         <v>37</v>
       </c>
-      <c r="R18" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -2061,7 +2055,7 @@
         <v>0.01</v>
       </c>
       <c r="Q19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T19" t="e">
         <v>#DIV/0!</v>
@@ -2080,9 +2074,7 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="I20" t="s">
         <v>21</v>
       </c>
@@ -2105,7 +2097,7 @@
         <v>0.05</v>
       </c>
       <c r="Q20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T20" t="e">
         <v>#DIV/0!</v>

</xml_diff>

<commit_message>
added decaying step lr
</commit_message>
<xml_diff>
--- a/model_notes.xlsx
+++ b/model_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfels\OneDrive\Dokumenter\vae_lung_tumor_segmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D03FD1-AE72-4478-A2A4-73134AECD6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB6B6FA-30A0-4BEA-BC4F-F507998A423B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="46">
   <si>
     <t>No.</t>
   </si>
@@ -140,12 +140,33 @@
   </si>
   <si>
     <t>Fits on dev set - mistake</t>
+  </si>
+  <si>
+    <t>1e-3 (step 5, gamma 0.5)</t>
+  </si>
+  <si>
+    <t>1e-3 (step 10, gamma 0.5)</t>
+  </si>
+  <si>
+    <t>1e-3 (step 5, gamma 0.9)</t>
+  </si>
+  <si>
+    <t>1.5e-3 (step 7, gamma 0.9)</t>
+  </si>
+  <si>
+    <t>Either increase step and gamma, try adding dense layers or increase kld loss by a little bit to ensure the latent space is aranged nicely</t>
+  </si>
+  <si>
+    <t>2e-3 (step 7, gamma 0.95)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -623,9 +644,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Farve1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,7 +1014,7 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.5546875" bestFit="1" customWidth="1"/>
@@ -1005,7 +1027,7 @@
     <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2107,6 +2129,51 @@
       <c r="A21">
         <v>32</v>
       </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21">
+        <v>0.30559999999999998</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21">
+        <v>256</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21">
+        <v>64</v>
+      </c>
+      <c r="O21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21">
+        <v>0.05</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>37</v>
+      </c>
       <c r="T21" t="e">
         <v>#DIV/0!</v>
       </c>
@@ -2115,20 +2182,160 @@
       <c r="A22">
         <v>33</v>
       </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22">
+        <v>0.3049</v>
+      </c>
+      <c r="G22">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>256</v>
+      </c>
+      <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22">
+        <v>64</v>
+      </c>
+      <c r="O22" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22">
+        <v>0.05</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>34</v>
       </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <v>256</v>
+      </c>
+      <c r="K23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23">
+        <v>64</v>
+      </c>
+      <c r="O23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23">
+        <v>0.05</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>35</v>
       </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.30349999999999999</v>
+      </c>
+      <c r="G24">
+        <v>79</v>
+      </c>
+      <c r="I24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24">
+        <v>256</v>
+      </c>
+      <c r="K24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24">
+        <v>64</v>
+      </c>
+      <c r="O24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24">
+        <v>0.05</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>